<commit_message>
Added the excel file for every tests of the webservice predicates
</commit_message>
<xml_diff>
--- a/Documentation/Tests/Logical/Test_WebService_Predicates.xlsx
+++ b/Documentation/Tests/Logical/Test_WebService_Predicates.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago\Documents\LAPR5\Documentation\Tests\Logical\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,17 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="63">
   <si>
     <t>Area</t>
   </si>
   <si>
-    <t>[Area Description]</t>
-  </si>
-  <si>
-    <t>[Goal description]</t>
-  </si>
-  <si>
     <t>Goal</t>
   </si>
   <si>
@@ -50,9 +44,6 @@
     <t>Expected result</t>
   </si>
   <si>
-    <t>Result</t>
-  </si>
-  <si>
     <t>Coluna1</t>
   </si>
   <si>
@@ -63,13 +54,172 @@
   </si>
   <si>
     <t>Coluna4</t>
+  </si>
+  <si>
+    <t>Logic WebService</t>
+  </si>
+  <si>
+    <t>Test of a fiew predicates of webservice to understand the feedback of the results</t>
+  </si>
+  <si>
+    <t>manual</t>
+  </si>
+  <si>
+    <t>webservice</t>
+  </si>
+  <si>
+    <t>http://uvm061.dei.isep.ipp.pt:5000/create_connection?personA=Artur&amp;personB=Nando&amp;strenght=1</t>
+  </si>
+  <si>
+    <t>"connection created"</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>On this queue of tests we pretend verify the consistency of the call on the webservice for the knowledge basis. This webservice is called a lot of times on the application, so it's convenient that the results are what we expect and eventually fix some bugs</t>
+  </si>
+  <si>
+    <t>"connection not created"</t>
+  </si>
+  <si>
+    <t>http://uvm061.dei.isep.ipp.pt:5000/remove_connection?personA=Artur&amp;personB=Nando</t>
+  </si>
+  <si>
+    <t>"connection removed"</t>
+  </si>
+  <si>
+    <t>http://uvm061.dei.isep.ipp.pt:5000/update_connection_strenght?personA=Tiago&amp;personB=Stephanie&amp;strenght=3</t>
+  </si>
+  <si>
+    <t>"connection edited"</t>
+  </si>
+  <si>
+    <t>http://uvm061.dei.isep.ipp.pt:5000/update_connection_tag?personA=Tiago&amp;personB=Stephanie&amp;tag=music</t>
+  </si>
+  <si>
+    <t>http://uvm061.dei.isep.ipp.pt:5000/remove_connection_tag?personA=Tiago&amp;personB=Stephanie&amp;tag=dog</t>
+  </si>
+  <si>
+    <t>http://uvm061.dei.isep.ipp.pt:5000/get_nodes?user=Tiago</t>
+  </si>
+  <si>
+    <t>List of every connections of user Tiago</t>
+  </si>
+  <si>
+    <t>http://uvm061.dei.isep.ipp.pt:5000/get_path?user=Tiago</t>
+  </si>
+  <si>
+    <t>Complete graph of user Tiago</t>
+  </si>
+  <si>
+    <t>http://uvm061.dei.isep.ipp.pt:5000/get_users</t>
+  </si>
+  <si>
+    <t>http://uvm061.dei.isep.ipp.pt:5000/get_users_dimension</t>
+  </si>
+  <si>
+    <t>List of every users ("nodes") of the graph</t>
+  </si>
+  <si>
+    <t>List of every users of the graph and the total number of connection of each user (dimension)</t>
+  </si>
+  <si>
+    <t>http://uvm061.dei.isep.ipp.pt:5000/get_users_strenght</t>
+  </si>
+  <si>
+    <t>List of every users of the graph and the total number of the strenght of the connections of each user</t>
+  </si>
+  <si>
+    <t>http://uvm061.dei.isep.ipp.pt:5000/get_tag_count</t>
+  </si>
+  <si>
+    <t>List every tags and the total number that each tag is used</t>
+  </si>
+  <si>
+    <t>http://uvm061.dei.isep.ipp.pt:5000/get_user_tag_count?user=Tiago</t>
+  </si>
+  <si>
+    <t>List containing every tags used on the connections of this user and the number of times that is used</t>
+  </si>
+  <si>
+    <t>Friend requested successfully</t>
+  </si>
+  <si>
+    <t>http://uvm061.dei.isep.ipp.pt:5000/request_friend?personA=Nando&amp;personB=Tiago</t>
+  </si>
+  <si>
+    <t>Friend game requested successfully</t>
+  </si>
+  <si>
+    <t>http://uvm061.dei.isep.ipp.pt:5000/game_response?personA=Tiago&amp;personB=Nando</t>
+  </si>
+  <si>
+    <t>Friend accepted successfully</t>
+  </si>
+  <si>
+    <t>http://uvm061.dei.isep.ipp.pt:5000/accept_response?personA=Nando&amp;personB=Tiago</t>
+  </si>
+  <si>
+    <t>http://uvm061.dei.isep.ipp.pt:5000/check_requests?user=Catarina</t>
+  </si>
+  <si>
+    <t>http://uvm061.dei.isep.ipp.pt:5000/check_game_requests?user=Tiago</t>
+  </si>
+  <si>
+    <t>List of every users that invite to play minigames to user Tiago</t>
+  </si>
+  <si>
+    <t>http://uvm061.dei.isep.ipp.pt:5000/check_friend_notifications?user=Tiago</t>
+  </si>
+  <si>
+    <t>List of every requests (pending or not) of user Catarina</t>
+  </si>
+  <si>
+    <t>List of every friendship requests sent to user Tiago</t>
+  </si>
+  <si>
+    <t>Friend request removed successfully</t>
+  </si>
+  <si>
+    <t>http://uvm061.dei.isep.ipp.pt:5000/remove_request?personA=Tiago&amp;personB=Nando</t>
+  </si>
+  <si>
+    <t>http://uvm061.dei.isep.ipp.pt:5000/get_all_tags</t>
+  </si>
+  <si>
+    <t>List of every tags used on graph of all users</t>
+  </si>
+  <si>
+    <t>http://uvm061.dei.isep.ipp.pt:5000/get_all_pending_requests?user=Tiago</t>
+  </si>
+  <si>
+    <t>List of every pending requests (send or received) of that user</t>
+  </si>
+  <si>
+    <t>Word added successfully</t>
+  </si>
+  <si>
+    <t>http://uvm061.dei.isep.ipp.pt:5000/add_word_hangman?word=Test</t>
+  </si>
+  <si>
+    <t>http://uvm061.dei.isep.ipp.pt:5000/get_common_graph?personA=Tiago&amp;personB=Stephanie</t>
+  </si>
+  <si>
+    <t>List of every common paths of user Tiago and user Stephanie</t>
+  </si>
+  <si>
+    <t>http://uvm061.dei.isep.ipp.pt:5000/get_user_added</t>
+  </si>
+  <si>
+    <t>List a random word existing on knowledge basis on the category user_added</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,6 +230,27 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -107,16 +278,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Cor3" xfId="1" builtinId="37"/>
+    <cellStyle name="Hiperligação" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -186,8 +366,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabela4" displayName="Tabela4" ref="B9:E25" totalsRowShown="0">
-  <autoFilter ref="B9:E25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabela4" displayName="Tabela4" ref="B9:E38" totalsRowShown="0">
+  <autoFilter ref="B9:E38"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Coluna1"/>
     <tableColumn id="2" name="Coluna2"/>
@@ -461,32 +641,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B9:E13"/>
+  <dimension ref="B9:E42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="32" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="104.42578125" customWidth="1"/>
+    <col min="4" max="4" width="91.140625" customWidth="1"/>
+    <col min="5" max="5" width="122.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
         <v>9</v>
-      </c>
-      <c r="C9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
@@ -494,41 +674,427 @@
         <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>8</v>
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" t="s">
+        <v>38</v>
+      </c>
+      <c r="E26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D30" t="s">
+        <v>49</v>
+      </c>
+      <c r="E30" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D31" t="s">
+        <v>47</v>
+      </c>
+      <c r="E31" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D32" t="s">
+        <v>50</v>
+      </c>
+      <c r="E32" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D34" t="s">
+        <v>54</v>
+      </c>
+      <c r="E34" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D35" t="s">
+        <v>56</v>
+      </c>
+      <c r="E35" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>13</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>16</v>
+      </c>
+      <c r="C42" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C16" r:id="rId1"/>
+    <hyperlink ref="C17" r:id="rId2"/>
+    <hyperlink ref="C18" r:id="rId3"/>
+    <hyperlink ref="C19" r:id="rId4"/>
+    <hyperlink ref="C20" r:id="rId5"/>
+    <hyperlink ref="C21" r:id="rId6"/>
+    <hyperlink ref="C22" r:id="rId7"/>
+    <hyperlink ref="C23" r:id="rId8"/>
+    <hyperlink ref="C24" r:id="rId9"/>
+    <hyperlink ref="C25" r:id="rId10"/>
+    <hyperlink ref="C26" r:id="rId11"/>
+    <hyperlink ref="C27" r:id="rId12"/>
+    <hyperlink ref="C28" r:id="rId13"/>
+    <hyperlink ref="C29" r:id="rId14"/>
+    <hyperlink ref="C30" r:id="rId15"/>
+    <hyperlink ref="C31" r:id="rId16"/>
+    <hyperlink ref="C32" r:id="rId17"/>
+    <hyperlink ref="C33" r:id="rId18"/>
+    <hyperlink ref="C34" r:id="rId19"/>
+    <hyperlink ref="C35" r:id="rId20"/>
+    <hyperlink ref="C36" r:id="rId21"/>
+    <hyperlink ref="C37" r:id="rId22"/>
+    <hyperlink ref="C38" r:id="rId23"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId24"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId25"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>